<commit_message>
Adding ResourceID column to handle ambiguity when resources have the same name
</commit_message>
<xml_diff>
--- a/Scripts/Policies/Tags/Tags_Resources.xlsx
+++ b/Scripts/Policies/Tags/Tags_Resources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repo\Azure\Scripts\Policies\Tags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6F7843-4484-4B18-8E2D-CD68DF37CF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE105E4-6E73-421F-8E32-2227DC9EDDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E23A1899-E413-4A68-ABC6-4D1ABD802009}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Resources and Tags" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Resources and Tags'!$B$1:$AH$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Resources and Tags'!$C$1:$AI$39</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +44,7 @@
     <author>Marcus Gaspar</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{1FDB0F67-FE2D-43DC-A4A4-60D495DEF395}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{1FDB0F67-FE2D-43DC-A4A4-60D495DEF395}">
       <text>
         <r>
           <rPr>
@@ -68,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{01AFD274-A5BC-4359-B157-051BD80ACF67}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{01AFD274-A5BC-4359-B157-051BD80ACF67}">
       <text>
         <r>
           <rPr>
@@ -92,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{8569B0DA-02D6-42CF-915E-70F239E2BCE7}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{8569B0DA-02D6-42CF-915E-70F239E2BCE7}">
       <text>
         <r>
           <rPr>
@@ -116,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{CBB9D4D9-07EF-4496-89AF-F4FBCCAB2C9C}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{CBB9D4D9-07EF-4496-89AF-F4FBCCAB2C9C}">
       <text>
         <r>
           <rPr>
@@ -140,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{8CD980DA-4256-488C-8C12-2583DFB4F354}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{8CD980DA-4256-488C-8C12-2583DFB4F354}">
       <text>
         <r>
           <rPr>
@@ -164,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{F934B6D9-57C9-4B4C-84B9-C9CF7142AD09}">
+    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{F934B6D9-57C9-4B4C-84B9-C9CF7142AD09}">
       <text>
         <r>
           <rPr>
@@ -188,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{79B603EE-35AF-4BC7-B060-7F2B2FAC39A6}">
+    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{79B603EE-35AF-4BC7-B060-7F2B2FAC39A6}">
       <text>
         <r>
           <rPr>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
   <si>
     <t>BMDB_Support Scope</t>
   </si>
@@ -318,9 +318,6 @@
     <t>Subscription</t>
   </si>
   <si>
-    <t>CAAZU1VALEDB023</t>
-  </si>
-  <si>
     <t>QA</t>
   </si>
   <si>
@@ -348,18 +345,9 @@
     <t>rg-hub-spoke</t>
   </si>
   <si>
-    <t>vm-arc-onprem-win1</t>
-  </si>
-  <si>
-    <t>rg-arc-onprem</t>
-  </si>
-  <si>
     <t>ME-MngEnvMCAP312459-marcusga-1</t>
   </si>
   <si>
-    <t>Canada Central1</t>
-  </si>
-  <si>
     <t>Canada Central2</t>
   </si>
   <si>
@@ -369,13 +357,34 @@
     <t>gaspar</t>
   </si>
   <si>
-    <t>Base Metals New 1</t>
-  </si>
-  <si>
     <t>Base Metals New 2</t>
   </si>
   <si>
-    <t>Base Metals New 3</t>
+    <t>ResourceID</t>
+  </si>
+  <si>
+    <t>ArcBox-SQL</t>
+  </si>
+  <si>
+    <t>rg-arc-it-pro</t>
+  </si>
+  <si>
+    <t>CAAZU1VALEDB026</t>
+  </si>
+  <si>
+    <t>Base Metals New 1a</t>
+  </si>
+  <si>
+    <t>Canada Central1a</t>
+  </si>
+  <si>
+    <t>CAAZU1VALEDB023a</t>
+  </si>
+  <si>
+    <t>Virtual Machine SQL2</t>
+  </si>
+  <si>
+    <t>SQL Server2</t>
   </si>
 </sst>
 </file>
@@ -788,462 +797,494 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:AH39"/>
+  <dimension ref="A1:AI39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" customWidth="1"/>
-    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" customWidth="1"/>
-    <col min="7" max="7" width="29.44140625" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.88671875" customWidth="1"/>
-    <col min="18" max="18" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="49.44140625" customWidth="1"/>
-    <col min="21" max="21" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="38.109375" customWidth="1"/>
-    <col min="24" max="24" width="46.88671875" customWidth="1"/>
-    <col min="25" max="25" width="23" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="29.5546875" customWidth="1"/>
-    <col min="28" max="28" width="26.109375" customWidth="1"/>
-    <col min="29" max="29" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21" customWidth="1"/>
-    <col min="32" max="32" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="34.109375" customWidth="1"/>
-    <col min="34" max="34" width="22" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" customWidth="1"/>
+    <col min="8" max="8" width="29.44140625" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.88671875" customWidth="1"/>
+    <col min="19" max="19" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="49.44140625" customWidth="1"/>
+    <col min="22" max="22" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="38.109375" customWidth="1"/>
+    <col min="25" max="25" width="46.88671875" customWidth="1"/>
+    <col min="26" max="26" width="23" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.5546875" customWidth="1"/>
+    <col min="29" max="29" width="26.109375" customWidth="1"/>
+    <col min="30" max="30" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21" customWidth="1"/>
+    <col min="33" max="33" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="34.109375" customWidth="1"/>
+    <col min="35" max="35" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" t="s">
-        <v>49</v>
-      </c>
-      <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="Z2" s="1"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" t="s">
-        <v>49</v>
-      </c>
-      <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
+      <c r="AB3" s="1"/>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
         <v>44</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
         <v>45</v>
       </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>49</v>
-      </c>
-      <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
-      <c r="AC4" s="1"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="X5" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AD4" s="1"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" t="s">
+        <v>45</v>
+      </c>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="X6" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AD5" s="1"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
-      <c r="AC6" s="1"/>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="X7" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AD6" s="1"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="X8" s="1"/>
+      <c r="AB7" s="1"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="W9" s="1"/>
+      <c r="AB8" s="1"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
-      <c r="AC9" s="1"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="W10" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AD9" s="1"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="W11" s="1"/>
+      <c r="AB10" s="1"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="W16" s="1"/>
+      <c r="AB11" s="1"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
-    </row>
-    <row r="17" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="X17" s="1"/>
+      <c r="AB16" s="1"/>
+    </row>
+    <row r="17" spans="21:30" x14ac:dyDescent="0.3">
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
-      <c r="AC17" s="1"/>
-    </row>
-    <row r="18" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="T18" s="1"/>
-      <c r="W18" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AD17" s="1"/>
+    </row>
+    <row r="18" spans="21:30" x14ac:dyDescent="0.3">
+      <c r="U18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
-    </row>
-    <row r="19" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="W19" s="1"/>
+      <c r="AB18" s="1"/>
+    </row>
+    <row r="19" spans="21:30" x14ac:dyDescent="0.3">
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
-    </row>
-    <row r="20" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="W20" s="1"/>
+      <c r="AB19" s="1"/>
+    </row>
+    <row r="20" spans="21:30" x14ac:dyDescent="0.3">
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
-    </row>
-    <row r="21" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="X21" s="1"/>
+      <c r="AB20" s="1"/>
+    </row>
+    <row r="21" spans="21:30" x14ac:dyDescent="0.3">
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
-    </row>
-    <row r="22" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="X22" s="1"/>
+      <c r="AB21" s="1"/>
+    </row>
+    <row r="22" spans="21:30" x14ac:dyDescent="0.3">
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
-    </row>
-    <row r="23" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="X23" s="1"/>
+      <c r="AB22" s="1"/>
+    </row>
+    <row r="23" spans="21:30" x14ac:dyDescent="0.3">
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
-    </row>
-    <row r="24" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="X24" s="1"/>
+      <c r="AB23" s="1"/>
+    </row>
+    <row r="24" spans="21:30" x14ac:dyDescent="0.3">
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
-    </row>
-    <row r="25" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="X25" s="1"/>
+      <c r="AB24" s="1"/>
+    </row>
+    <row r="25" spans="21:30" x14ac:dyDescent="0.3">
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
-    </row>
-    <row r="26" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="X26" s="1"/>
+      <c r="AB25" s="1"/>
+    </row>
+    <row r="26" spans="21:30" x14ac:dyDescent="0.3">
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
-    </row>
-    <row r="27" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="X27" s="1"/>
+      <c r="AB26" s="1"/>
+    </row>
+    <row r="27" spans="21:30" x14ac:dyDescent="0.3">
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
-    </row>
-    <row r="28" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="X28" s="1"/>
+      <c r="AB27" s="1"/>
+    </row>
+    <row r="28" spans="21:30" x14ac:dyDescent="0.3">
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
-    </row>
-    <row r="29" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="X29" s="1"/>
+      <c r="AB28" s="1"/>
+    </row>
+    <row r="29" spans="21:30" x14ac:dyDescent="0.3">
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
-      <c r="AC29" s="1"/>
-    </row>
-    <row r="30" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="X30" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AD29" s="1"/>
+    </row>
+    <row r="30" spans="21:30" x14ac:dyDescent="0.3">
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
-    </row>
-    <row r="31" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="X31" s="1"/>
+      <c r="AB30" s="1"/>
+    </row>
+    <row r="31" spans="21:30" x14ac:dyDescent="0.3">
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
-      <c r="AC31" s="1"/>
-    </row>
-    <row r="32" spans="20:29" x14ac:dyDescent="0.3">
-      <c r="X32" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AD31" s="1"/>
+    </row>
+    <row r="32" spans="21:30" x14ac:dyDescent="0.3">
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
-    </row>
-    <row r="33" spans="23:34" x14ac:dyDescent="0.3">
-      <c r="X33" s="1"/>
+      <c r="AB32" s="1"/>
+    </row>
+    <row r="33" spans="24:35" x14ac:dyDescent="0.3">
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
-    </row>
-    <row r="34" spans="23:34" x14ac:dyDescent="0.3">
-      <c r="X34" s="1"/>
+      <c r="AB33" s="1"/>
+    </row>
+    <row r="34" spans="24:35" x14ac:dyDescent="0.3">
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
-      <c r="AF34" s="1"/>
+      <c r="AB34" s="1"/>
       <c r="AG34" s="1"/>
       <c r="AH34" s="1"/>
-    </row>
-    <row r="35" spans="23:34" x14ac:dyDescent="0.3">
-      <c r="X35" s="1"/>
+      <c r="AI34" s="1"/>
+    </row>
+    <row r="35" spans="24:35" x14ac:dyDescent="0.3">
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
-      <c r="AF35" s="1"/>
+      <c r="AB35" s="1"/>
       <c r="AG35" s="1"/>
       <c r="AH35" s="1"/>
-    </row>
-    <row r="36" spans="23:34" x14ac:dyDescent="0.3">
-      <c r="W36" s="1"/>
+      <c r="AI35" s="1"/>
+    </row>
+    <row r="36" spans="24:35" x14ac:dyDescent="0.3">
       <c r="X36" s="1"/>
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
-      <c r="AC36" s="1"/>
-    </row>
-    <row r="37" spans="23:34" x14ac:dyDescent="0.3">
-      <c r="X37" s="1"/>
+      <c r="AB36" s="1"/>
+      <c r="AD36" s="1"/>
+    </row>
+    <row r="37" spans="24:35" x14ac:dyDescent="0.3">
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
-    </row>
-    <row r="38" spans="23:34" x14ac:dyDescent="0.3">
-      <c r="X38" s="1"/>
+      <c r="AB37" s="1"/>
+    </row>
+    <row r="38" spans="24:35" x14ac:dyDescent="0.3">
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
-    </row>
-    <row r="39" spans="23:34" x14ac:dyDescent="0.3">
-      <c r="X39" s="1"/>
+      <c r="AB38" s="1"/>
+    </row>
+    <row r="39" spans="24:35" x14ac:dyDescent="0.3">
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
+      <c r="AB39" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:AH39" xr:uid="{FEDF7DB2-D7EA-4479-98E9-E4FCE09FCAF7}"/>
+  <autoFilter ref="C1:AI39" xr:uid="{FEDF7DB2-D7EA-4479-98E9-E4FCE09FCAF7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>